<commit_message>
add validasi format register perujuk
</commit_message>
<xml_diff>
--- a/backend/public/format/formatRegistrasiPerujuk.xlsx
+++ b/backend/public/format/formatRegistrasiPerujuk.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="17970" windowHeight="9750"/>
+    <workbookView windowWidth="14460" windowHeight="7770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>no</t>
   </si>
@@ -34,6 +34,9 @@
     <t>nama</t>
   </si>
   <si>
+    <t>no hp</t>
+  </si>
+  <si>
     <t>nik</t>
   </si>
   <si>
@@ -89,6 +92,12 @@
   </si>
   <si>
     <t>PNS</t>
+  </si>
+  <si>
+    <t>annisa</t>
+  </si>
+  <si>
+    <t>085437321</t>
   </si>
   <si>
     <t>6371030905900003</t>
@@ -117,10 +126,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
+    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="23">
     <font>
@@ -158,11 +167,40 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -174,14 +212,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -190,7 +236,22 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -198,14 +259,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -213,7 +267,29 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -226,73 +302,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -303,43 +312,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -351,7 +450,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -363,127 +492,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -494,6 +503,65 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -515,58 +583,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -585,155 +603,146 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="26" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="18" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="16" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="22" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="32" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="6" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="7" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="8" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="8" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" applyNumberFormat="false" applyFont="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="26" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="14" borderId="5" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="false" applyFill="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="24" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="0" fontId="18" fillId="18" borderId="6" applyNumberFormat="false" applyAlignment="false" applyProtection="false">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="false" applyFill="false" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -754,6 +763,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="true"/>
     <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" quotePrefix="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="58" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="true" applyFont="true" applyFill="true" applyBorder="true" applyAlignment="true" quotePrefix="true"/>
   </cellXfs>
   <cellStyles count="50">
@@ -1075,10 +1087,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:V2"/>
+  <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:V2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.75" outlineLevelRow="1"/>
@@ -1088,21 +1100,21 @@
     <col min="3" max="3" width="12.2866666666667" customWidth="true"/>
     <col min="4" max="4" width="16.7133333333333" customWidth="true"/>
     <col min="5" max="5" width="8.28666666666667" customWidth="true"/>
-    <col min="6" max="6" width="18.7133333333333" customWidth="true"/>
-    <col min="7" max="7" width="18.5733333333333" customWidth="true"/>
-    <col min="8" max="8" width="12.8533333333333" customWidth="true"/>
-    <col min="12" max="12" width="14.8533333333333" customWidth="true"/>
-    <col min="13" max="13" width="15.5733333333333" customWidth="true"/>
-    <col min="14" max="14" width="12.8533333333333" customWidth="true"/>
-    <col min="15" max="15" width="13.14" customWidth="true"/>
-    <col min="17" max="17" width="16.4266666666667" customWidth="true"/>
-    <col min="18" max="18" width="12.7133333333333" customWidth="true"/>
-    <col min="19" max="19" width="12.14" customWidth="true"/>
-    <col min="21" max="21" width="12.4266666666667" customWidth="true"/>
-    <col min="22" max="22" width="11.8533333333333" customWidth="true"/>
+    <col min="6" max="7" width="18.7133333333333" customWidth="true"/>
+    <col min="8" max="8" width="18.5733333333333" customWidth="true"/>
+    <col min="9" max="9" width="12.8533333333333" customWidth="true"/>
+    <col min="13" max="13" width="14.8533333333333" customWidth="true"/>
+    <col min="14" max="14" width="15.5733333333333" customWidth="true"/>
+    <col min="15" max="15" width="12.8533333333333" customWidth="true"/>
+    <col min="16" max="16" width="13.14" customWidth="true"/>
+    <col min="18" max="18" width="16.4266666666667" customWidth="true"/>
+    <col min="19" max="19" width="12.7133333333333" customWidth="true"/>
+    <col min="20" max="20" width="12.14" customWidth="true"/>
+    <col min="22" max="22" width="12.4266666666667" customWidth="true"/>
+    <col min="23" max="23" width="11.8533333333333" customWidth="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1169,70 +1181,78 @@
       <c r="V1" t="s">
         <v>21</v>
       </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:22">
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C2" s="3">
         <v>1009</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
         <v>25</v>
       </c>
+      <c r="F2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="G2" s="6" t="s">
+        <v>27</v>
+      </c>
       <c r="H2" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J2" s="3">
+        <v>28</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L2" s="4">
+      <c r="K2" s="3">
+        <v>30</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="4">
         <v>100000000</v>
       </c>
-      <c r="M2" s="4">
+      <c r="N2" s="4">
         <v>100000</v>
       </c>
-      <c r="N2" s="4">
+      <c r="O2" s="4">
         <v>10000</v>
       </c>
-      <c r="O2" s="4">
+      <c r="P2" s="4">
         <v>100000</v>
       </c>
-      <c r="P2" s="1" t="s">
+      <c r="Q2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="R2" s="3">
+      <c r="R2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="S2" s="3">
         <v>1000000</v>
       </c>
-      <c r="S2" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="T2" s="3">
+      <c r="T2" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="U2" s="3">
         <v>1</v>
       </c>
-      <c r="U2" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="V2" s="1">
+      <c r="V2" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="W2" s="1">
         <v>1000</v>
       </c>
     </row>

</xml_diff>